<commit_message>
Add update of 03/12
</commit_message>
<xml_diff>
--- a/Halite 2/src/Halite Helper.xlsx
+++ b/Halite 2/src/Halite Helper.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>x</t>
   </si>
@@ -51,6 +51,33 @@
   </si>
   <si>
     <t>Diff</t>
+  </si>
+  <si>
+    <t>samples</t>
+  </si>
+  <si>
+    <t>won</t>
+  </si>
+  <si>
+    <t>lost</t>
+  </si>
+  <si>
+    <t>lower bound</t>
+  </si>
+  <si>
+    <t>upper bound</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>stddev</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>std</t>
   </si>
 </sst>
 </file>
@@ -402,14 +429,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -429,10 +458,10 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>98.73</v>
+        <v>152.99</v>
       </c>
       <c r="C2">
-        <v>75.13</v>
+        <v>87.06</v>
       </c>
       <c r="D2">
         <v>0.5</v>
@@ -442,7 +471,7 @@
       </c>
       <c r="G2">
         <f>SQRT(B4+C4)</f>
-        <v>3.4489563638874912</v>
+        <v>3.2223749005973832</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -450,10 +479,10 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>100.2</v>
+        <v>154</v>
       </c>
       <c r="C3">
-        <v>78.25</v>
+        <v>84</v>
       </c>
       <c r="D3">
         <v>0.5</v>
@@ -463,7 +492,7 @@
       </c>
       <c r="G3">
         <f>G2-D2-D3</f>
-        <v>2.4489563638874912</v>
+        <v>2.2223749005973832</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -472,11 +501,11 @@
       </c>
       <c r="B4">
         <f>(B3-B2)^2</f>
-        <v>2.1608999999999967</v>
+        <v>1.0200999999999816</v>
       </c>
       <c r="C4">
         <f>(C3-C2)^2</f>
-        <v>9.7344000000000293</v>
+        <v>9.3636000000000141</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
@@ -486,13 +515,89 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D6">
-        <v>11.34</v>
-      </c>
-      <c r="E6">
-        <f>4+6.92</f>
-        <v>10.92</v>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <f>B7-B8</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <f>B8/B7</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f>B12-B10*SQRT(B12*(1-B12)/B7)</f>
+        <v>0.42469227056401648</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f>B12+B10*SQRT(B12*(1-B12)/B7)</f>
+        <v>0.77530772943598347</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>47.56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <f>B17-3*B18</f>
+        <v>46.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add v15, rank 14th
</commit_message>
<xml_diff>
--- a/Halite 2/src/Halite Helper.xlsx
+++ b/Halite 2/src/Halite Helper.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>x</t>
   </si>
@@ -78,13 +78,32 @@
   </si>
   <si>
     <t>std</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Percentile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="173" formatCode="0.0000000000000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,14 +129,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -429,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,6 +463,7 @@
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -458,10 +482,10 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>152.99</v>
+        <v>227.93770000000001</v>
       </c>
       <c r="C2">
-        <v>87.06</v>
+        <v>109.8947</v>
       </c>
       <c r="D2">
         <v>0.5</v>
@@ -469,9 +493,9 @@
       <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <f>SQRT(B4+C4)</f>
-        <v>3.2223749005973832</v>
+        <v>12.281006460384273</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -479,20 +503,20 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>154</v>
+        <v>217.3869</v>
       </c>
       <c r="C3">
-        <v>84</v>
+        <v>103.6095</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>9.84</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <f>G2-D2-D3</f>
-        <v>2.2223749005973832</v>
+        <v>1.9410064603842727</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -501,18 +525,18 @@
       </c>
       <c r="B4">
         <f>(B3-B2)^2</f>
-        <v>1.0200999999999816</v>
+        <v>111.3193806400002</v>
       </c>
       <c r="C4">
         <f>(C3-C2)^2</f>
-        <v>9.3636000000000141</v>
+        <v>39.503739040000042</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
       </c>
       <c r="G4">
         <f>D2+D3</f>
-        <v>1</v>
+        <v>10.34</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -528,7 +552,7 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -537,7 +561,7 @@
       </c>
       <c r="B9">
         <f>B7-B8</f>
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -552,27 +576,27 @@
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <f>B8/B7</f>
-        <v>0.6</v>
+        <v>0.76666666666666672</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <f>B12-B10*SQRT(B12*(1-B12)/B7)</f>
-        <v>0.42469227056401648</v>
+        <v>0.61531502802830074</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <f>B12+B10*SQRT(B12*(1-B12)/B7)</f>
-        <v>0.77530772943598347</v>
+        <v>0.9180183053050327</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -580,7 +604,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>47.56</v>
+        <v>49.19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +612,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -597,7 +621,32 @@
       </c>
       <c r="B19">
         <f>B17-3*B18</f>
-        <v>46.06</v>
+        <v>48.29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>2313</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1">
+        <f>B21/B22</f>
+        <v>6.0527453523562475E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>